<commit_message>
Test: Implement Visual Encoder Warmup for VLM tests
</commit_message>
<xml_diff>
--- a/tests/artifacts/Jarvis_Benchmark_Report.xlsx
+++ b/tests/artifacts/Jarvis_Benchmark_Report.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="LLM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="VLM" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -689,4 +690,201 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Loadout</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Scenario</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>TTFT (s)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>TPS</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>VRAM Peak (GB)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>base-qwen30-multi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>bunny</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.3603103999994346</v>
+      </c>
+      <c r="E2" t="n">
+        <v>126.5041844137252</v>
+      </c>
+      <c r="F2" t="n">
+        <v>24.1025390625</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>The animal in the video is a large, white, anthropomorphic rabbit. It is shown in a series of scenes in a lush, green field.
+- In the first scene, the rabbit is lying on its back on the grass, with a large, pink butterfly resting on its belly.
+- In the second scene, the rabbit is sitting up, looking down at the butterfly, which is now perched on its head.
+- In the final scene, the rabbit is standing in a field, looking down at a small, red, round object on the ground, possibly a flower or a ball.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>base-qwen30-multi</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>jarvis_logo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1563606999989133</v>
+      </c>
+      <c r="E3" t="n">
+        <v>176.0141120761007</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24.1025390625</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>This image features a stylized, futuristic robot head, which appears to be a representation of Iron Man's helmet. The helmet is centrally positioned within a circular, high-tech interface that resembles a heads-up display (HUD) or targeting system.
+Key visual elements include:
+- A glowing blue, metallic helmet with a sleek, angular design.
+- Bright, glowing green eyes that give it an intense, focused look.
+- Red accents on the sides of the helmet, possibly representing earpieces or sensors.
+- A circular frame surrounding the helmet, composed of concentric rings with glowing blue lines and markings, suggesting a digital or scanning interface.
+- The overall color scheme is dominated by shades of blue and black, creating a dark, high-tech, and cybernetic atmosphere.
+The image is likely a logo or icon for a game, app, or digital platform related to Iron Man or a similar sci-fi theme.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>base-qwen30-multi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>three_objects</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1310329000043566</v>
+      </c>
+      <c r="E4" t="n">
+        <v>146.9501913408375</v>
+      </c>
+      <c r="F4" t="n">
+        <v>24.1025390625</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Based on the image provided, we can identify the following:
+- There is one red circle in the upper left.
+- There is one blue circle in the upper right.
+- There is one green circle in the lower center.
+Each of these is a distinct, colored circle.
+Therefore, there are 3 colored circles in the photo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>base-qwen30-multi</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>traffic</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1.030388999999559</v>
+      </c>
+      <c r="E5" t="n">
+        <v>39.32765441986089</v>
+      </c>
+      <c r="F5" t="n">
+        <v>24.1025390625</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Based on the video frames provided, the following types of vehicles are visible:
+- **Car**: A white car is seen driving into the parking lot and then parking.
+- **Bicycle**: A person is seen riding a bicycle across the parking lot.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>